<commit_message>
Updated The Browser Invoke Setup also Updated Test HomePage,LoginPage and LoginPageWithDDT.
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tejas\Nop Ecommerce Project With Robot Framework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791F72D1-761D-454F-BA81-8211FD23224C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E268A762-C484-4606-8BB6-49EAE69AC207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
-  <si>
-    <t>Status</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>${Email}</t>
   </si>
@@ -49,33 +46,6 @@
   </si>
   <si>
     <t>admin@your.com</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Test Number</t>
-  </si>
-  <si>
-    <t>Objective</t>
-  </si>
-  <si>
-    <t>1) Go to website
-2) Inspect and click on "Email" &amp; "Password" element.
-3) Enter Valid Email but Invalid Password.</t>
-  </si>
-  <si>
-    <t>1) Go to website
-2) Inspect and click on "Email" &amp; "Password" element.
-3) Enter Invalid Email but Valid Password.</t>
-  </si>
-  <si>
-    <t>1) Go to website
-2) Inspect and click on "Email" &amp; "Password" element.
-3) Enter Invalid Email and Password.</t>
   </si>
 </sst>
 </file>
@@ -113,7 +83,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -122,10 +92,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -143,107 +128,12 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -286,61 +176,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -623,100 +480,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" style="18" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
+    <row r="1" spans="1:2" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>0</v>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="13" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:A5"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{080DA7BB-1BD9-47FE-B1E6-FF04A4945561}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{7E2AFBA5-2925-45F9-9FA0-5C387EDD47AC}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{80AEAE0C-4669-43F6-9D70-45C6DAFBEC37}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{080DA7BB-1BD9-47FE-B1E6-FF04A4945561}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{7E2AFBA5-2925-45F9-9FA0-5C387EDD47AC}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{80AEAE0C-4669-43F6-9D70-45C6DAFBEC37}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>